<commit_message>
Revert "Update Feiertage.xlsx" (in order to work on that in a separate branch)
This reverts commit 28d8c47e83524b593420fc7f2014c322564c343a.
</commit_message>
<xml_diff>
--- a/lpagg/resources_load/Feiertage.xlsx
+++ b/lpagg/resources_load/Feiertage.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lv\Documents\GitHub\lpagg\lpagg\resources_load\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\MA\2_Projekte\SIZ10015_futureSuN\4_Bearbeitung\AP4_Transformation\AP404_Konzepte für zukünftige Systemlösungen\Lastprofile\VDI 4655\Berechnung\Typtage\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
   <si>
     <t>! --- VDI 4655 --- Holiday Calendar --------------------------------------------</t>
   </si>
@@ -34,46 +34,67 @@
     <t>! All other rows can contain holidays from the years you want to calculate.</t>
   </si>
   <si>
+    <t xml:space="preserve">! Holidays were taken from http://www.feiertage.info/ </t>
+  </si>
+  <si>
     <t>Feiertag</t>
   </si>
   <si>
     <t>Datum</t>
   </si>
   <si>
+    <t>Neujahr</t>
+  </si>
+  <si>
+    <t>Karfreitag</t>
+  </si>
+  <si>
+    <t>Ostersonntag</t>
+  </si>
+  <si>
+    <t>Ostermontag</t>
+  </si>
+  <si>
+    <t>Maifeiertag</t>
+  </si>
+  <si>
+    <t>Christi Himmelfahrt</t>
+  </si>
+  <si>
+    <t>Pfingstsonntag</t>
+  </si>
+  <si>
+    <t>Pfingstmontag</t>
+  </si>
+  <si>
+    <t>Fronleichnam</t>
+  </si>
+  <si>
+    <t>Tag der deutschen Einheit</t>
+  </si>
+  <si>
+    <t>Reformationstag</t>
+  </si>
+  <si>
+    <t>Allerheiligen</t>
+  </si>
+  <si>
+    <t>1. Weihnachtstag</t>
+  </si>
+  <si>
+    <t>2. Weihnachtstag</t>
+  </si>
+  <si>
+    <t>Heilige 3 Könige</t>
+  </si>
+  <si>
+    <t>Mariä Himmelfahrt</t>
+  </si>
+  <si>
+    <t>Buß und Bettag</t>
+  </si>
+  <si>
     <t>! The first row contains the headers  'Datum' and  'Feiertag'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Neujahr</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Karfreitag</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ostermontag</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Maifeiertag</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Christi Himmelfahrt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pfingstmontag</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tag der Deutschen Einheit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Reformationstag</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1. Weihnachtstag</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2. Weihnachtstag</t>
-  </si>
-  <si>
-    <t>! Holidays were taken from https://www.feiertage.net/frei-tage.php for northern Germany (Lower Saxony, Hamburg, Bremen, Schleswig Holstein, Mecklenburg Western Pomerania, Brandenburg)</t>
   </si>
 </sst>
 </file>
@@ -882,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,15 +916,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42736</v>
+        <v>42005</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -911,231 +932,231 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>42839</v>
+        <v>42010</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>42842</v>
+        <v>42097</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>42856</v>
+        <v>42099</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>42880</v>
+        <v>42100</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>42891</v>
+        <v>42125</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43011</v>
+        <v>42138</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43039</v>
+        <v>42148</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43094</v>
+        <v>42149</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43095</v>
+        <v>42159</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43101</v>
+        <v>42231</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43189</v>
+        <v>42280</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>43192</v>
+        <v>42308</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>43221</v>
+        <v>42309</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>43230</v>
+        <v>42326</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>43241</v>
+        <v>42363</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>43376</v>
+        <v>42364</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>43404</v>
+        <v>42370</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>43459</v>
+        <v>42736</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>43460</v>
+        <v>42741</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>43466</v>
+        <v>42839</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>43574</v>
+        <v>42841</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>43577</v>
+        <v>42842</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>43586</v>
+        <v>42856</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>43615</v>
+        <v>42880</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>43626</v>
+        <v>42890</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>43741</v>
+        <v>42891</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>43769</v>
+        <v>42901</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>43824</v>
+        <v>42962</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>43825</v>
+        <v>43011</v>
       </c>
       <c r="B31" t="s">
         <v>16</v>
@@ -1143,242 +1164,186 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>43831</v>
+        <v>43039</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>43931</v>
+        <v>43040</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>43934</v>
+        <v>43061</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>43952</v>
+        <v>43094</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>43972</v>
+        <v>43095</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>43983</v>
+        <v>43101</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>44107</v>
+        <v>43106</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>44135</v>
+        <v>43189</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>44190</v>
+        <v>43191</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>44191</v>
+        <v>43192</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>44197</v>
+        <v>43221</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>44288</v>
+        <v>43230</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>44291</v>
+        <v>43240</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>44317</v>
+        <v>43241</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>44329</v>
+        <v>43251</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>44340</v>
+        <v>43327</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>44472</v>
+        <v>43376</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>44500</v>
+        <v>43404</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>44555</v>
+        <v>43405</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>44556</v>
+        <v>43425</v>
       </c>
       <c r="B51" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>44562</v>
+        <v>43459</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>44666</v>
+        <v>43460</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>44669</v>
+        <v>43466</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>44682</v>
-      </c>
-      <c r="B55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>44707</v>
-      </c>
-      <c r="B56" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>44718</v>
-      </c>
-      <c r="B57" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>44837</v>
-      </c>
-      <c r="B58" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>44865</v>
-      </c>
-      <c r="B59" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>44920</v>
-      </c>
-      <c r="B60" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>44921</v>
-      </c>
-      <c r="B61" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1391,7 +1356,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1378,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -1423,7 +1388,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>